<commit_message>
Pushing batch files, setting batch name in config.properties
</commit_message>
<xml_diff>
--- a/src/test/resources/Team12_TechRockstarts_Lms_data.xlsx
+++ b/src/test/resources/Team12_TechRockstarts_Lms_data.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uvaraj/eclipse-workspace/Team12_TechRockstars_LMS_UI_Phase2/src/test/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498D8038-3653-0543-A460-8ACC2A78BD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="3200" windowWidth="27240" windowHeight="16440" xr2:uid="{A0D0EEA0-6D56-934A-97A5-96C05BA695CA}"/>
+    <workbookView xWindow="4700" yWindow="3200" windowWidth="27240" windowHeight="16420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="programData" sheetId="1" r:id="rId1"/>
+    <sheet name="batch" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>dataKey</t>
   </si>
@@ -80,16 +75,80 @@
   </si>
   <si>
     <t>java for sdets</t>
+  </si>
+  <si>
+    <t>scenario</t>
+  </si>
+  <si>
+    <t>batch-suffix</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>no-of-classes</t>
+  </si>
+  <si>
+    <t>error-message</t>
+  </si>
+  <si>
+    <t>VALID</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>INVALID-BATCH-SUFFIX</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>This field accept only numbers and max 5 count.</t>
+  </si>
+  <si>
+    <t>INVALID-MISSING-MANDATORY-FIELD</t>
+  </si>
+  <si>
+    <t>Number of classes is required.</t>
+  </si>
+  <si>
+    <t>VALID-MANDATORY-FIELDS</t>
+  </si>
+  <si>
+    <t>VALID-MANDATORY-FIELDS-CANCEL</t>
+  </si>
+  <si>
+    <t>Showing 0 to 0 of 0 entries</t>
+  </si>
+  <si>
+    <t>VALID-EDIT</t>
+  </si>
+  <si>
+    <t>Successful</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,8 +174,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -177,7 +238,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -229,7 +290,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -423,28 +484,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F63DDEE-03C9-B540-B11C-1BD0ADF980F3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -469,7 +530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -483,7 +544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -491,13 +552,144 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5"/>
+  <cols>
+    <col min="1" max="1" width="19.9140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1">
+        <v>179</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>179</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>183</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>210</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1">
+        <v>183</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Pushing batch files, setting batch name in config.properties (#22)
</commit_message>
<xml_diff>
--- a/src/test/resources/Team12_TechRockstarts_Lms_data.xlsx
+++ b/src/test/resources/Team12_TechRockstarts_Lms_data.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uvaraj/eclipse-workspace/Team12_TechRockstars_LMS_UI_Phase2/src/test/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498D8038-3653-0543-A460-8ACC2A78BD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="3200" windowWidth="27240" windowHeight="16440" xr2:uid="{A0D0EEA0-6D56-934A-97A5-96C05BA695CA}"/>
+    <workbookView xWindow="4700" yWindow="3200" windowWidth="27240" windowHeight="16420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="programData" sheetId="1" r:id="rId1"/>
+    <sheet name="batch" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>dataKey</t>
   </si>
@@ -80,16 +75,80 @@
   </si>
   <si>
     <t>java for sdets</t>
+  </si>
+  <si>
+    <t>scenario</t>
+  </si>
+  <si>
+    <t>batch-suffix</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>no-of-classes</t>
+  </si>
+  <si>
+    <t>error-message</t>
+  </si>
+  <si>
+    <t>VALID</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>INVALID-BATCH-SUFFIX</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>This field accept only numbers and max 5 count.</t>
+  </si>
+  <si>
+    <t>INVALID-MISSING-MANDATORY-FIELD</t>
+  </si>
+  <si>
+    <t>Number of classes is required.</t>
+  </si>
+  <si>
+    <t>VALID-MANDATORY-FIELDS</t>
+  </si>
+  <si>
+    <t>VALID-MANDATORY-FIELDS-CANCEL</t>
+  </si>
+  <si>
+    <t>Showing 0 to 0 of 0 entries</t>
+  </si>
+  <si>
+    <t>VALID-EDIT</t>
+  </si>
+  <si>
+    <t>Successful</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,8 +174,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -177,7 +238,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -229,7 +290,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -423,28 +484,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F63DDEE-03C9-B540-B11C-1BD0ADF980F3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -469,7 +530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -483,7 +544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -491,13 +552,144 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5"/>
+  <cols>
+    <col min="1" max="1" width="19.9140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1">
+        <v>179</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>179</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>183</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>210</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1">
+        <v>183</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>